<commit_message>
updated antonio feed files
</commit_message>
<xml_diff>
--- a/Antonio-Feed/_LNA SN Datasheets/LNF LNA Shipments .xlsx
+++ b/Antonio-Feed/_LNA SN Datasheets/LNF LNA Shipments .xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/_LNA SN Datasheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD01EA7E-83D9-0A48-9D5F-21F8076D9722}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="96" windowWidth="16260" windowHeight="8208"/>
+    <workbookView xWindow="63340" yWindow="460" windowWidth="28300" windowHeight="19740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>Comments</t>
   </si>
@@ -376,17 +382,60 @@
                      (F) Fraunhofer</t>
     </r>
   </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0027A_v2</t>
+  </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0032A_v2</t>
+  </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0058A_v2</t>
+  </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0066A_v2</t>
+  </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0067A_v2</t>
+  </si>
+  <si>
+    <t>LNF-ABLNC1_15A sn0098A_v2</t>
+  </si>
+  <si>
+    <t>C-0027F</t>
+  </si>
+  <si>
+    <t>C-0032F</t>
+  </si>
+  <si>
+    <t>C-0058F</t>
+  </si>
+  <si>
+    <t>C-0066F</t>
+  </si>
+  <si>
+    <t>C-0067F</t>
+  </si>
+  <si>
+    <t>C-0098F</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -737,7 +786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,167 +794,170 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -929,6 +981,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -977,7 +1032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1010,9 +1065,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1045,6 +1117,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1220,45 +1309,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I53"/>
+  <dimension ref="B1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="1"/>
-    <col min="2" max="2" width="2.77734375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="4.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="20.77734375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.21875" customWidth="1"/>
+    <col min="1" max="1" width="2.83203125" customWidth="1"/>
+    <col min="2" max="2" width="2.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="4.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" customWidth="1"/>
     <col min="9" max="9" width="25.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="D1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="2:9" ht="25.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="43" t="s">
+    <row r="2" spans="2:9" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="I2" s="28"/>
     </row>
-    <row r="3" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
         <v>81</v>
       </c>
@@ -1281,7 +1370,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>1</v>
       </c>
@@ -1297,10 +1386,10 @@
       <c r="F4" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="45"/>
+      <c r="G4" s="43"/>
       <c r="I4" s="58"/>
     </row>
-    <row r="5" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="7"/>
       <c r="C5" s="18"/>
       <c r="D5" s="8">
@@ -1312,10 +1401,10 @@
       <c r="F5" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="46"/>
+      <c r="G5" s="44"/>
       <c r="I5" s="58"/>
     </row>
-    <row r="6" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="7"/>
       <c r="C6" s="18"/>
       <c r="D6" s="8">
@@ -1327,10 +1416,10 @@
       <c r="F6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="46"/>
+      <c r="G6" s="44"/>
       <c r="I6" s="58"/>
     </row>
-    <row r="7" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="10"/>
       <c r="C7" s="19"/>
       <c r="D7" s="11">
@@ -1342,9 +1431,9 @@
       <c r="F7" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="47"/>
-    </row>
-    <row r="8" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G7" s="45"/>
+    </row>
+    <row r="8" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="7">
         <v>2</v>
       </c>
@@ -1360,12 +1449,12 @@
       <c r="F8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="48"/>
+      <c r="G8" s="56"/>
       <c r="I8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="7"/>
       <c r="C9" s="18"/>
       <c r="D9" s="8">
@@ -1377,9 +1466,9 @@
       <c r="F9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="49"/>
-    </row>
-    <row r="10" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="57"/>
+    </row>
+    <row r="10" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="7"/>
       <c r="C10" s="18"/>
       <c r="D10" s="9">
@@ -1391,9 +1480,9 @@
       <c r="F10" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="46"/>
-    </row>
-    <row r="11" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G10" s="44"/>
+    </row>
+    <row r="11" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="10"/>
       <c r="C11" s="19"/>
       <c r="D11" s="11">
@@ -1405,9 +1494,9 @@
       <c r="F11" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="47"/>
-    </row>
-    <row r="12" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7">
         <v>3</v>
       </c>
@@ -1423,12 +1512,12 @@
       <c r="F12" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="50"/>
+      <c r="G12" s="46"/>
       <c r="I12" s="30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
       <c r="C13" s="18"/>
       <c r="D13" s="8">
@@ -1440,9 +1529,9 @@
       <c r="F13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="51"/>
-    </row>
-    <row r="14" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="47"/>
+    </row>
+    <row r="14" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="C14" s="18"/>
       <c r="D14" s="8">
@@ -1454,9 +1543,9 @@
       <c r="F14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="46"/>
-    </row>
-    <row r="15" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G14" s="44"/>
+    </row>
+    <row r="15" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="7"/>
       <c r="C15" s="18"/>
       <c r="D15" s="8">
@@ -1468,9 +1557,9 @@
       <c r="F15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="46"/>
-    </row>
-    <row r="16" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G15" s="44"/>
+    </row>
+    <row r="16" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7"/>
       <c r="C16" s="18"/>
       <c r="D16" s="8">
@@ -1482,9 +1571,9 @@
       <c r="F16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="46"/>
-    </row>
-    <row r="17" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="44"/>
+    </row>
+    <row r="17" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7"/>
       <c r="C17" s="18"/>
       <c r="D17" s="8">
@@ -1496,9 +1585,9 @@
       <c r="F17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="G17" s="46"/>
-    </row>
-    <row r="18" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="44"/>
+    </row>
+    <row r="18" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
       <c r="C18" s="18"/>
       <c r="D18" s="8">
@@ -1510,9 +1599,9 @@
       <c r="F18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="46"/>
-    </row>
-    <row r="19" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="44"/>
+    </row>
+    <row r="19" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="18"/>
       <c r="D19" s="8">
@@ -1524,9 +1613,9 @@
       <c r="F19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="G19" s="46"/>
-    </row>
-    <row r="20" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G19" s="44"/>
+    </row>
+    <row r="20" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="18"/>
       <c r="D20" s="26">
@@ -1538,11 +1627,11 @@
       <c r="F20" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="G20" s="52" t="s">
+      <c r="G20" s="48" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="18"/>
       <c r="D21" s="8">
@@ -1554,9 +1643,9 @@
       <c r="F21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="46"/>
-    </row>
-    <row r="22" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="44"/>
+    </row>
+    <row r="22" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="21">
         <v>4</v>
       </c>
@@ -1572,14 +1661,14 @@
       <c r="F22" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="53" t="s">
+      <c r="G22" s="49" t="s">
         <v>102</v>
       </c>
       <c r="I22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="18"/>
       <c r="D23" s="8">
@@ -1591,9 +1680,9 @@
       <c r="F23" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="46"/>
-    </row>
-    <row r="24" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G23" s="44"/>
+    </row>
+    <row r="24" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="18"/>
       <c r="D24" s="8">
@@ -1605,9 +1694,9 @@
       <c r="F24" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="46"/>
-    </row>
-    <row r="25" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G24" s="44"/>
+    </row>
+    <row r="25" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="18"/>
       <c r="D25" s="8">
@@ -1619,9 +1708,9 @@
       <c r="F25" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="46"/>
-    </row>
-    <row r="26" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G25" s="44"/>
+    </row>
+    <row r="26" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="18"/>
       <c r="D26" s="8">
@@ -1633,9 +1722,9 @@
       <c r="F26" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="46"/>
-    </row>
-    <row r="27" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G26" s="44"/>
+    </row>
+    <row r="27" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="18"/>
       <c r="D27" s="8">
@@ -1647,9 +1736,9 @@
       <c r="F27" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="46"/>
-    </row>
-    <row r="28" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G27" s="44"/>
+    </row>
+    <row r="28" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="18"/>
       <c r="D28" s="8">
@@ -1661,9 +1750,9 @@
       <c r="F28" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G28" s="46"/>
-    </row>
-    <row r="29" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G28" s="44"/>
+    </row>
+    <row r="29" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="18"/>
       <c r="D29" s="8">
@@ -1675,9 +1764,9 @@
       <c r="F29" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="G29" s="46"/>
-    </row>
-    <row r="30" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G29" s="44"/>
+    </row>
+    <row r="30" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="18"/>
       <c r="D30" s="8">
@@ -1689,9 +1778,9 @@
       <c r="F30" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="46"/>
-    </row>
-    <row r="31" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="44"/>
+    </row>
+    <row r="31" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="18"/>
       <c r="D31" s="8">
@@ -1703,9 +1792,9 @@
       <c r="F31" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="G31" s="46"/>
-    </row>
-    <row r="32" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G31" s="44"/>
+    </row>
+    <row r="32" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="21">
         <v>5</v>
       </c>
@@ -1721,12 +1810,12 @@
       <c r="F32" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="54"/>
+      <c r="G32" s="50"/>
       <c r="I32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="18"/>
       <c r="D33" s="8">
@@ -1738,12 +1827,12 @@
       <c r="F33" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="G33" s="46"/>
+      <c r="G33" s="44"/>
       <c r="I33" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="18"/>
       <c r="D34" s="29">
@@ -1755,9 +1844,9 @@
       <c r="F34" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="G34" s="55"/>
-    </row>
-    <row r="35" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="51"/>
+    </row>
+    <row r="35" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
       <c r="C35" s="18"/>
       <c r="D35" s="8">
@@ -1769,9 +1858,9 @@
       <c r="F35" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="G35" s="46"/>
-    </row>
-    <row r="36" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="44"/>
+    </row>
+    <row r="36" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="7"/>
       <c r="C36" s="18"/>
       <c r="D36" s="8">
@@ -1783,9 +1872,9 @@
       <c r="F36" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="G36" s="46"/>
-    </row>
-    <row r="37" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="44"/>
+    </row>
+    <row r="37" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="7"/>
       <c r="C37" s="18"/>
       <c r="D37" s="8">
@@ -1797,9 +1886,9 @@
       <c r="F37" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="G37" s="46"/>
-    </row>
-    <row r="38" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="44"/>
+    </row>
+    <row r="38" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="7"/>
       <c r="C38" s="18"/>
       <c r="D38" s="8">
@@ -1811,9 +1900,9 @@
       <c r="F38" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="G38" s="46"/>
-    </row>
-    <row r="39" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G38" s="44"/>
+    </row>
+    <row r="39" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="7"/>
       <c r="C39" s="18"/>
       <c r="D39" s="29">
@@ -1825,9 +1914,9 @@
       <c r="F39" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="G39" s="55"/>
-    </row>
-    <row r="40" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="51"/>
+    </row>
+    <row r="40" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="7"/>
       <c r="C40" s="18"/>
       <c r="D40" s="8">
@@ -1839,9 +1928,9 @@
       <c r="F40" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="G40" s="46"/>
-    </row>
-    <row r="41" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G40" s="44"/>
+    </row>
+    <row r="41" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="7"/>
       <c r="C41" s="18"/>
       <c r="D41" s="8">
@@ -1853,17 +1942,17 @@
       <c r="F41" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="G41" s="46"/>
-    </row>
-    <row r="42" spans="2:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="44"/>
+    </row>
+    <row r="42" spans="2:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="7"/>
       <c r="C42" s="18"/>
       <c r="D42" s="8"/>
       <c r="E42" s="8"/>
       <c r="F42" s="40"/>
-      <c r="G42" s="46"/>
-    </row>
-    <row r="43" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G42" s="44"/>
+    </row>
+    <row r="43" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B43" s="21">
         <v>6</v>
       </c>
@@ -1879,12 +1968,12 @@
       <c r="F43" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="56"/>
+      <c r="G43" s="52"/>
       <c r="I43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B44" s="7"/>
       <c r="C44" s="18"/>
       <c r="D44" s="8">
@@ -1896,12 +1985,12 @@
       <c r="F44" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="G44" s="55"/>
+      <c r="G44" s="51"/>
       <c r="I44" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B45" s="7"/>
       <c r="C45" s="18"/>
       <c r="D45" s="8">
@@ -1913,9 +2002,9 @@
       <c r="F45" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="G45" s="46"/>
-    </row>
-    <row r="46" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G45" s="44"/>
+    </row>
+    <row r="46" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B46" s="7"/>
       <c r="C46" s="18"/>
       <c r="D46" s="8">
@@ -1927,9 +2016,9 @@
       <c r="F46" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="G46" s="46"/>
-    </row>
-    <row r="47" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G46" s="44"/>
+    </row>
+    <row r="47" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="7"/>
       <c r="C47" s="18"/>
       <c r="D47" s="8">
@@ -1941,9 +2030,9 @@
       <c r="F47" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="G47" s="46"/>
-    </row>
-    <row r="48" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G47" s="44"/>
+    </row>
+    <row r="48" spans="2:9" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="7"/>
       <c r="C48" s="18"/>
       <c r="D48" s="8">
@@ -1955,9 +2044,9 @@
       <c r="F48" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="G48" s="46"/>
-    </row>
-    <row r="49" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G48" s="44"/>
+    </row>
+    <row r="49" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B49" s="7"/>
       <c r="C49" s="18"/>
       <c r="D49" s="8">
@@ -1969,9 +2058,9 @@
       <c r="F49" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="G49" s="46"/>
-    </row>
-    <row r="50" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G49" s="44"/>
+    </row>
+    <row r="50" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="7"/>
       <c r="C50" s="18"/>
       <c r="D50" s="8">
@@ -1983,9 +2072,9 @@
       <c r="F50" s="39" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="46"/>
-    </row>
-    <row r="51" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G50" s="44"/>
+    </row>
+    <row r="51" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B51" s="7"/>
       <c r="C51" s="18"/>
       <c r="D51" s="8">
@@ -1997,9 +2086,9 @@
       <c r="F51" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="G51" s="46"/>
-    </row>
-    <row r="52" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G51" s="44"/>
+    </row>
+    <row r="52" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B52" s="7"/>
       <c r="C52" s="18"/>
       <c r="D52" s="8">
@@ -2011,15 +2100,111 @@
       <c r="F52" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="G52" s="46"/>
-    </row>
-    <row r="53" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G52" s="44"/>
+    </row>
+    <row r="53" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="15"/>
       <c r="C53" s="20"/>
       <c r="D53" s="16"/>
       <c r="E53" s="16"/>
       <c r="F53" s="42"/>
-      <c r="G53" s="57"/>
+      <c r="G53" s="53"/>
+    </row>
+    <row r="54" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B54" s="21">
+        <v>7</v>
+      </c>
+      <c r="C54" s="25">
+        <v>44280</v>
+      </c>
+      <c r="D54" s="23">
+        <v>1</v>
+      </c>
+      <c r="E54" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="F54" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="G54" s="52"/>
+    </row>
+    <row r="55" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B55" s="7"/>
+      <c r="C55" s="18"/>
+      <c r="D55" s="8">
+        <v>2</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F55" s="39" t="s">
+        <v>113</v>
+      </c>
+      <c r="G55" s="51"/>
+    </row>
+    <row r="56" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B56" s="7"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="8">
+        <v>3</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F56" s="39" t="s">
+        <v>114</v>
+      </c>
+      <c r="G56" s="44"/>
+    </row>
+    <row r="57" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B57" s="7"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="8">
+        <v>4</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="G57" s="44"/>
+    </row>
+    <row r="58" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B58" s="7"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="8">
+        <v>5</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="F58" s="59" t="s">
+        <v>116</v>
+      </c>
+      <c r="G58" s="44"/>
+    </row>
+    <row r="59" spans="2:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="B59" s="7"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="8">
+        <v>6</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="G59" s="44"/>
+    </row>
+    <row r="60" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="15"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2033,24 +2218,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>